<commit_message>
csv for nov 23 US stock
</commit_message>
<xml_diff>
--- a/US_stocks_231103.xlsx
+++ b/US_stocks_231103.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19635" windowHeight="7695"/>
+    <workbookView windowWidth="19635" windowHeight="7695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LargeCap" sheetId="2" r:id="rId1"/>
@@ -1924,16 +1924,16 @@
   <sheetPr/>
   <dimension ref="B1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="B1" sqref="$A1:$XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="3" width="9" style="1"/>
     <col min="4" max="4" width="42.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.25" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="24.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" style="1" customWidth="1"/>
     <col min="9" max="10" width="9" style="1"/>
@@ -3251,8 +3251,8 @@
   <sheetPr/>
   <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>